<commit_message>
BOM updates and minor DRC fixes
</commit_message>
<xml_diff>
--- a/bom/master_v1.xlsx
+++ b/bom/master_v1.xlsx
@@ -19,6 +19,7 @@
     <definedName name="FFC">Mouser!$I$3</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
+  <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
   <si>
     <t>Description</t>
   </si>
@@ -213,12 +214,6 @@
     <t>Headers &amp; Wire Housings 2P SR UNSHRD HRD TIN OVER NI</t>
   </si>
   <si>
-    <t>Headers &amp; Wire Housings 3P SR UNSHRD HRD TIN OVER NI</t>
-  </si>
-  <si>
-    <t>649-68015-403HLF</t>
-  </si>
-  <si>
     <t>649-68021-408HLF</t>
   </si>
   <si>
@@ -229,6 +224,18 @@
   </si>
   <si>
     <t>649-77313-418-16LF</t>
+  </si>
+  <si>
+    <t>649-SFW16R-2STE1LF</t>
+  </si>
+  <si>
+    <t>FFC &amp; FPC Connectors 16P SIDE SMT ZIF UPPER CONTACT</t>
+  </si>
+  <si>
+    <t>Headers &amp; Wire Housings 2.54MM CGRIDIII HDR 3P R/A SR SEL AU</t>
+  </si>
+  <si>
+    <t>538-90121-0763</t>
   </si>
 </sst>
 </file>
@@ -631,10 +638,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B822EE0-7F50-4032-91A3-680B28449694}">
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -645,7 +652,7 @@
     <col min="4" max="4" width="8.88671875" style="1"/>
     <col min="5" max="5" width="17.77734375" style="4" customWidth="1"/>
     <col min="6" max="8" width="8.88671875" style="1"/>
-    <col min="9" max="9" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15" style="1" customWidth="1"/>
     <col min="10" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
@@ -684,17 +691,17 @@
       </c>
       <c r="D2" s="1">
         <f>BD*2</f>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E2" s="4">
         <f>C2*D2</f>
-        <v>2.04</v>
+        <v>3.4000000000000004</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>14</v>
       </c>
       <c r="I2" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -709,17 +716,17 @@
       </c>
       <c r="D3" s="1">
         <f>BD*2</f>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E3" s="4">
-        <f t="shared" ref="E3:E30" si="0">C3*D3</f>
-        <v>4.1399999999999997</v>
+        <f t="shared" ref="E3:E31" si="0">C3*D3</f>
+        <v>6.8999999999999995</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I3" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -734,11 +741,11 @@
       </c>
       <c r="D4" s="1">
         <f>1*BD</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E4" s="4">
         <f t="shared" si="0"/>
-        <v>0.66</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -753,18 +760,18 @@
       </c>
       <c r="D5" s="1">
         <f>3*BD</f>
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E5" s="4">
         <f t="shared" si="0"/>
-        <v>1.08</v>
+        <v>1.7999999999999998</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>43</v>
       </c>
       <c r="I5" s="8">
         <f>SUM(E:E)</f>
-        <v>55.614000000000004</v>
+        <v>104.99</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -779,11 +786,11 @@
       </c>
       <c r="D6" s="1">
         <f>1*BD</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E6" s="4">
         <f t="shared" si="0"/>
-        <v>0.84000000000000008</v>
+        <v>1.4000000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -798,11 +805,11 @@
       </c>
       <c r="D7" s="1">
         <f>1*BD</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E7" s="4">
         <f>C7*D7</f>
-        <v>0.96</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -817,11 +824,11 @@
       </c>
       <c r="D8" s="1">
         <f>1*BD</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E8" s="4">
         <f t="shared" si="0"/>
-        <v>0.69000000000000006</v>
+        <v>1.1500000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -836,11 +843,11 @@
       </c>
       <c r="D9" s="1">
         <f>1*BD</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E9" s="4">
         <f t="shared" si="0"/>
-        <v>0.33</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
@@ -855,11 +862,11 @@
       </c>
       <c r="D10" s="1">
         <f>BD*2</f>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E10" s="4">
         <f t="shared" si="0"/>
-        <v>3.7800000000000002</v>
+        <v>6.3</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
@@ -874,11 +881,11 @@
       </c>
       <c r="D11" s="1">
         <f>3*BD</f>
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E11" s="4">
         <f t="shared" si="0"/>
-        <v>1.89</v>
+        <v>3.15</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -893,11 +900,11 @@
       </c>
       <c r="D12" s="1">
         <f>1*BD</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E12" s="4">
         <f t="shared" si="0"/>
-        <v>0.92999999999999994</v>
+        <v>1.55</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -912,11 +919,11 @@
       </c>
       <c r="D13" s="1">
         <f>1*BD</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E13" s="4">
         <f t="shared" si="0"/>
-        <v>4.5600000000000005</v>
+        <v>7.6</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -931,11 +938,11 @@
       </c>
       <c r="D14" s="1">
         <f>1*BD</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E14" s="4">
         <f t="shared" si="0"/>
-        <v>3.1500000000000004</v>
+        <v>5.25</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -950,11 +957,11 @@
       </c>
       <c r="D15" s="1">
         <f>1*BD</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E15" s="4">
         <f t="shared" si="0"/>
-        <v>0.30000000000000004</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -969,11 +976,11 @@
       </c>
       <c r="D16" s="1">
         <f>4*BD</f>
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E16" s="4">
         <f t="shared" si="0"/>
-        <v>0.26400000000000001</v>
+        <v>0.43999999999999995</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -988,11 +995,11 @@
       </c>
       <c r="D17" s="1">
         <f>BD*2</f>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E17" s="4">
         <f t="shared" si="0"/>
-        <v>0.60000000000000009</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -1006,12 +1013,12 @@
         <v>0.1</v>
       </c>
       <c r="D18" s="1">
-        <f>1*BD</f>
-        <v>3</v>
+        <f t="shared" ref="D18:D23" si="1">1*BD</f>
+        <v>5</v>
       </c>
       <c r="E18" s="4">
         <f t="shared" si="0"/>
-        <v>0.30000000000000004</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -1025,12 +1032,12 @@
         <v>0.1</v>
       </c>
       <c r="D19" s="1">
-        <f>1*BD</f>
-        <v>3</v>
+        <f t="shared" si="1"/>
+        <v>5</v>
       </c>
       <c r="E19" s="4">
         <f t="shared" si="0"/>
-        <v>0.30000000000000004</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -1044,12 +1051,12 @@
         <v>0.1</v>
       </c>
       <c r="D20" s="1">
-        <f>1*BD</f>
-        <v>3</v>
+        <f t="shared" si="1"/>
+        <v>5</v>
       </c>
       <c r="E20" s="4">
         <f t="shared" si="0"/>
-        <v>0.30000000000000004</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -1063,12 +1070,12 @@
         <v>0.27</v>
       </c>
       <c r="D21" s="1">
-        <f>1*BD</f>
-        <v>3</v>
+        <f t="shared" si="1"/>
+        <v>5</v>
       </c>
       <c r="E21" s="4">
         <f t="shared" si="0"/>
-        <v>0.81</v>
+        <v>1.35</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -1082,12 +1089,12 @@
         <v>3.09</v>
       </c>
       <c r="D22" s="1">
-        <f>1*BD</f>
-        <v>3</v>
+        <f t="shared" si="1"/>
+        <v>5</v>
       </c>
       <c r="E22" s="4">
         <f t="shared" si="0"/>
-        <v>9.27</v>
+        <v>15.45</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -1101,12 +1108,12 @@
         <v>0.78</v>
       </c>
       <c r="D23" s="1">
-        <f>1*BD</f>
-        <v>3</v>
+        <f t="shared" si="1"/>
+        <v>5</v>
       </c>
       <c r="E23" s="4">
         <f t="shared" si="0"/>
-        <v>2.34</v>
+        <v>3.9000000000000004</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -1121,11 +1128,11 @@
       </c>
       <c r="D24" s="1">
         <f>BD*2</f>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E24" s="4">
         <f t="shared" si="0"/>
-        <v>8.4599999999999991</v>
+        <v>14.1</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -1139,12 +1146,12 @@
         <v>0.6</v>
       </c>
       <c r="D25" s="1">
-        <f>1*BD</f>
+        <f t="shared" ref="D25:D29" si="2">1*BD</f>
+        <v>5</v>
+      </c>
+      <c r="E25" s="4">
+        <f t="shared" si="0"/>
         <v>3</v>
-      </c>
-      <c r="E25" s="4">
-        <f t="shared" si="0"/>
-        <v>1.7999999999999998</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -1158,12 +1165,12 @@
         <v>0.52</v>
       </c>
       <c r="D26" s="1">
-        <f>1*BD</f>
-        <v>3</v>
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="E26" s="4">
         <f t="shared" si="0"/>
-        <v>1.56</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -1177,69 +1184,88 @@
         <v>0.18</v>
       </c>
       <c r="D27" s="1">
-        <f>1*BD</f>
-        <v>3</v>
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="E27" s="4">
         <f t="shared" si="0"/>
-        <v>0.54</v>
+        <v>0.89999999999999991</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="C28" s="4">
-        <v>0.27</v>
+        <v>0.75</v>
       </c>
       <c r="D28" s="1">
-        <f>1*BD</f>
-        <v>3</v>
+        <f>1*BD+1*FFC</f>
+        <v>10</v>
       </c>
       <c r="E28" s="4">
         <f t="shared" si="0"/>
-        <v>0.81</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C29" s="4">
         <v>0.47</v>
       </c>
       <c r="D29" s="1">
-        <f>1*BD</f>
-        <v>3</v>
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="E29" s="4">
         <f t="shared" si="0"/>
-        <v>1.41</v>
+        <v>2.3499999999999996</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C30" s="4">
         <v>0.5</v>
       </c>
       <c r="D30" s="1">
-        <f>1*BD</f>
-        <v>3</v>
+        <f>1*BD+1*FFC</f>
+        <v>10</v>
       </c>
       <c r="E30" s="4">
         <f t="shared" si="0"/>
-        <v>1.5</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C31" s="4">
+        <v>0.73</v>
+      </c>
+      <c r="D31" s="1">
+        <f>FFC*1</f>
+        <v>5</v>
+      </c>
+      <c r="E31" s="4">
+        <f t="shared" si="0"/>
+        <v>3.65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>